<commit_message>
Na duvida deste comit
</commit_message>
<xml_diff>
--- a/PlanoDisplay.xlsx
+++ b/PlanoDisplay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisco/Documents/GitHub/Estacao-Meteorologica-Arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5E5564-B0C4-0549-9BE2-77833C3731F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992814C0-7A33-E541-999E-152091278CA0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16000" yWindow="9880" windowWidth="20640" windowHeight="10680" xr2:uid="{815BA5BD-3D10-A34C-9751-92E23798B3DE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="17">
   <si>
     <t>H</t>
   </si>
@@ -88,10 +88,23 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,10 +151,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA93A35-8CD6-1146-8299-D1734C2336EC}">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:Y15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,7 +484,7 @@
     <col min="22" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>1</v>
@@ -532,7 +547,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -593,7 +608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -650,7 +665,7 @@
       </c>
       <c r="U3" s="1"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -701,7 +716,7 @@
       </c>
       <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -759,6 +774,300 @@
       <c r="U5" s="1" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3">
+        <v>4</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5</v>
+      </c>
+      <c r="G8" s="3">
+        <v>6</v>
+      </c>
+      <c r="H8" s="3">
+        <v>7</v>
+      </c>
+      <c r="I8" s="3">
+        <v>8</v>
+      </c>
+      <c r="J8" s="3">
+        <v>9</v>
+      </c>
+      <c r="K8" s="3">
+        <v>10</v>
+      </c>
+      <c r="L8" s="3">
+        <v>11</v>
+      </c>
+      <c r="M8" s="3">
+        <v>12</v>
+      </c>
+      <c r="N8" s="3">
+        <v>13</v>
+      </c>
+      <c r="O8" s="3">
+        <v>14</v>
+      </c>
+      <c r="P8" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>16</v>
+      </c>
+      <c r="R8" s="3">
+        <v>17</v>
+      </c>
+      <c r="S8" s="3">
+        <v>18</v>
+      </c>
+      <c r="T8" s="3">
+        <v>19</v>
+      </c>
+      <c r="U8" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>